<commit_message>
Implemented function nextTraceID and added auto update of timestamps
</commit_message>
<xml_diff>
--- a/database/metadata/data/sheets/data-format.xlsx
+++ b/database/metadata/data/sheets/data-format.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drraf\Documents\Privat\Development\Projects\appman-api-spec\database\metadata\data\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED18023-42D6-402D-AD73-8E3494016C75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3311E374-E409-4721-BDFC-2DB5A4D12FD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
   <si>
     <t>formatID</t>
   </si>
@@ -168,6 +168,18 @@
   </si>
   <si>
     <t>(?:yes|no)</t>
+  </si>
+  <si>
+    <t>phoneNumber</t>
+  </si>
+  <si>
+    <t>^\+[1-9]\d{1,14}$</t>
+  </si>
+  <si>
+    <t>bcrypt hash</t>
+  </si>
+  <si>
+    <t>^[$]2[abxy]?[$](?:0[4-9]|[12][0-9]|3[01])[$][./0-9a-zA-Z]{53}$</t>
   </si>
 </sst>
 </file>
@@ -488,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,7 +559,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <f t="shared" ref="A4:A25" si="0">A3+1</f>
+        <f t="shared" ref="A4:A27" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -686,13 +698,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="D13" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -701,13 +713,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="D14" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -716,7 +728,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>35</v>
@@ -731,7 +743,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>39</v>
@@ -746,7 +758,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>35</v>
@@ -761,7 +773,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>39</v>
@@ -776,7 +788,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>35</v>
@@ -791,7 +803,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>39</v>
@@ -806,13 +818,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D21" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -821,13 +833,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D22" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -836,13 +848,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D23" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -851,13 +863,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D24" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -866,12 +878,42 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D27" s="1">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added validations and fields to developer table
</commit_message>
<xml_diff>
--- a/database/metadata/data/sheets/data-format.xlsx
+++ b/database/metadata/data/sheets/data-format.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drraf\Documents\Privat\Development\Projects\appman-api-spec\database\metadata\data\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3311E374-E409-4721-BDFC-2DB5A4D12FD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B32CF7-B4E8-4A50-81A8-FB3A0CE63D92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -149,15 +149,9 @@
     <t>^(\d{4})-(\d{2})-(\d{2})T(\d{2}):(\d{2}):(\d{2}(?:\.\d*)?)((-(\d{2}):(\d{2})|Z)?)$</t>
   </si>
   <si>
-    <t>(?:[a-z0-9!#$%&amp;'*+/=?^_`{|}~-]+(?:\.[a-z0-9!#$%&amp;'*+/=?^_`{|}~-]+)*|"(?:[\x01-\x08\x0b\x0c\x0e-\x1f\x21\x23-\x5b\x5d-\x7f]|\\[\x01-\x09\x0b\x0c\x0e-\x7f])*")@(?:(?:[a-z0-9](?:[a-z0-9-]*[a-z0-9])?\.)+[a-z0-9](?:[a-z0-9-]*[a-z0-9])?|\[(?:(?:25[0-5]|2[0-4][0-9]|[01]?[0-9][0-9]?)\.){3}(?:25[0-5]|2[0-4][0-9]|[01]?[0-9][0-9]?|[a-z0-9-]*[a-z0-9]:(?:[\x01-\x08\x0b\x0c\x0e-\x1f\x21-\x5a\x53-\x7f]|\\[\x01-\x09\x0b\x0c\x0e-\x7f])+)\])</t>
-  </si>
-  <si>
     <t>^\d+$</t>
   </si>
   <si>
-    <t>(?=(.*[0-9]))(?=.*[\!@#$%^&amp;*()\\[\]{}\-_+=~`|:;"'&lt;&gt;,./?])(?=.*[a-z])(?=(.*[A-Z]))(?=(.*)).{8,}</t>
-  </si>
-  <si>
     <t>[-+]?([0-9]*[.])?[0-9]+([eE][-+]?\d+)?</t>
   </si>
   <si>
@@ -179,7 +173,13 @@
     <t>bcrypt hash</t>
   </si>
   <si>
-    <t>^[$]2[abxy]?[$](?:0[4-9]|[12][0-9]|3[01])[$][./0-9a-zA-Z]{53}$</t>
+    <t>(?:[a-z0-9!#$%&amp;'*+\/=?^_`{|}~-]+(?:\.[a-z0-9!#$%&amp;'*+\/=?^_`{|}~-]+)*|"(?:[\x01-\x08\x0b\x0c\x0e-\x1f\x21\x23-\x5b\x5d-\x7f]|\\[\x01-\x09\x0b\x0c\x0e-\x7f])*")@(?:(?:[a-z0-9](?:[a-z0-9-]*[a-z0-9])?\.)+[a-z0-9](?:[a-z0-9-]*[a-z0-9])?|\[(?:(?:25[0-5]|2[0-4][0-9]|[01]?[0-9][0-9]?)\.){3}(?:25[0-5]|2[0-4][0-9]|[01]?[0-9][0-9]?|[a-z0-9-]*[a-z0-9]:(?:[\x01-\x08\x0b\x0c\x0e-\x1f\x21-\x5a\x53-\x7f]|\\[\x01-\x09\x0b\x0c\x0e-\x7f])+)\])</t>
+  </si>
+  <si>
+    <t>^[$]2[abxy]?[$](?:0[4-9]|[12][0-9]|3[01])[$][.\/0-9a-zA-Z]{53}$</t>
+  </si>
+  <si>
+    <t>(?=(.*[0-9]))(?=.*[\!@#$%^&amp;*()\\[\]{}\-_+=~`|:;"'&lt;&gt;,.\/?])(?=.*[a-z])(?=(.*[A-Z]))(?=(.*)).{8,}</t>
   </si>
 </sst>
 </file>
@@ -503,7 +503,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,7 +626,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
@@ -686,7 +686,7 @@
         <v>14</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D12" s="1">
         <v>1</v>
@@ -698,10 +698,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D13" s="1">
         <v>1</v>
@@ -713,10 +713,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="D14" s="1">
         <v>1</v>
@@ -746,7 +746,7 @@
         <v>16</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D16" s="1">
         <v>2</v>
@@ -776,7 +776,7 @@
         <v>18</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D18" s="1">
         <v>2</v>
@@ -806,7 +806,7 @@
         <v>20</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D20" s="1">
         <v>2</v>
@@ -836,7 +836,7 @@
         <v>22</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D22" s="1">
         <v>2</v>
@@ -851,7 +851,7 @@
         <v>23</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D23" s="1">
         <v>3</v>
@@ -866,7 +866,7 @@
         <v>24</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D24" s="1">
         <v>3</v>
@@ -881,7 +881,7 @@
         <v>25</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D25" s="1">
         <v>4</v>
@@ -896,7 +896,7 @@
         <v>26</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D26" s="1">
         <v>4</v>
@@ -911,7 +911,7 @@
         <v>27</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D27" s="1">
         <v>4</v>

</xml_diff>